<commit_message>
Addition of readme file
</commit_message>
<xml_diff>
--- a/LSPA Buoy Sensor History.xlsx
+++ b/LSPA Buoy Sensor History.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steeleb\Dropbox\Lake Sunapee\monitoring\buoy data\programs\LSPA_buoy_GH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weathersk\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7490" windowHeight="1820"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t xml:space="preserve">This file documents the sensor history of the LSPA buoy for publication to EDI. </t>
+  </si>
+  <si>
+    <t>It was compiled by Bethel Steele, Kathleen Weathers' Laboratory, Cary Institute of Ecosystem Studies, February 2022</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -286,8 +289,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -295,7 +298,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -589,17 +592,22 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.9"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.9">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.9">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -617,18 +625,18 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="10.296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.390625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.10546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.60546875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="3"/>
+    <col min="7" max="16384" width="8.78515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.7">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -648,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -668,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -688,7 +696,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -708,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -728,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -748,7 +756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -768,7 +776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -788,7 +796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -808,7 +816,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -828,7 +836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -848,7 +856,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -882,17 +890,17 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="8" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.390625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.69921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.796875" style="3"/>
+    <col min="5" max="5" width="51.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.78515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -909,7 +917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -926,7 +934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -943,7 +951,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -960,7 +968,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -977,7 +985,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -994,7 +1002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1011,7 +1019,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1028,7 +1036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1053,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1062,7 +1070,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1126,15 +1134,15 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="18.59765625" customWidth="1"/>
-    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="18.60546875" customWidth="1"/>
+    <col min="5" max="5" width="10.390625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.390625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="16" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -1155,7 +1163,7 @@
       </c>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
@@ -1176,7 +1184,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A3" s="10" t="s">
         <v>34</v>
       </c>
@@ -1197,7 +1205,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A4" s="10" t="s">
         <v>34</v>
       </c>
@@ -1218,7 +1226,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
@@ -1239,7 +1247,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A6" s="10" t="s">
         <v>34</v>
       </c>
@@ -1260,7 +1268,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>

</xml_diff>